<commit_message>
refined: data structure for the InputParser
</commit_message>
<xml_diff>
--- a/Documents/NecessaryDataForParser.xlsx
+++ b/Documents/NecessaryDataForParser.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="56">
   <si>
     <t>Место</t>
   </si>
@@ -178,30 +178,6 @@
     <t>позавчера</t>
   </si>
   <si>
-    <t>эту</t>
-  </si>
-  <si>
-    <t>недел</t>
-  </si>
-  <si>
-    <t>+</t>
-  </si>
-  <si>
-    <t>+у</t>
-  </si>
-  <si>
-    <t>+ов</t>
-  </si>
-  <si>
-    <t>+ю</t>
-  </si>
-  <si>
-    <t>-</t>
-  </si>
-  <si>
-    <t>+е</t>
-  </si>
-  <si>
     <t>предыдущий</t>
   </si>
   <si>
@@ -209,6 +185,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>Простое</t>
+  </si>
+  <si>
+    <t>Составное</t>
+  </si>
+  <si>
+    <t>Мат. Соответствие</t>
   </si>
 </sst>
 </file>
@@ -455,16 +440,13 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -504,6 +486,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -832,10 +817,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z33"/>
+  <dimension ref="A1:Z35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -843,14 +828,17 @@
     <col min="1" max="16384" width="10.28515625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="72" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="2"/>
+      <c r="C1" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" s="11"/>
       <c r="F1" s="7" t="s">
         <v>29</v>
       </c>
@@ -872,7 +860,7 @@
       <c r="L1" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="M1" s="23" t="s">
+      <c r="M1" s="22" t="s">
         <v>26</v>
       </c>
       <c r="N1" s="7" t="s">
@@ -896,19 +884,19 @@
       <c r="T1" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="U1" s="23" t="s">
+      <c r="U1" s="22" t="s">
         <v>20</v>
       </c>
       <c r="W1" s="2"/>
-      <c r="X1" s="25"/>
+      <c r="X1" s="24"/>
     </row>
     <row r="2" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="9" t="s">
+      <c r="A2" s="11"/>
+      <c r="B2" s="11"/>
+      <c r="C2" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="11"/>
       <c r="F2" s="7" t="s">
         <v>30</v>
       </c>
@@ -944,12 +932,12 @@
       </c>
     </row>
     <row r="3" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="9" t="s">
+      <c r="A3" s="11"/>
+      <c r="B3" s="11"/>
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="11"/>
       <c r="E3" s="7">
         <v>0</v>
       </c>
@@ -983,24 +971,26 @@
       <c r="W3" s="3"/>
     </row>
     <row r="4" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="C4" s="9" t="s">
+      <c r="A4" s="11"/>
+      <c r="B4" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="C4" s="11" t="s">
         <v>14</v>
       </c>
+      <c r="D4" s="11"/>
       <c r="E4" s="7" t="s">
         <v>10</v>
       </c>
       <c r="W4" s="3"/>
     </row>
     <row r="5" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="13"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="3" t="s">
+      <c r="A5" s="11"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11" t="s">
         <v>24</v>
       </c>
+      <c r="D5" s="11"/>
       <c r="E5" s="7" t="s">
         <v>12</v>
       </c>
@@ -1045,11 +1035,12 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="13"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="3" t="s">
+      <c r="A6" s="11"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11" t="s">
         <v>16</v>
       </c>
+      <c r="D6" s="11"/>
       <c r="H6" s="7" t="s">
         <v>28</v>
       </c>
@@ -1082,10 +1073,11 @@
       </c>
     </row>
     <row r="7" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="13"/>
-      <c r="C7" s="12" t="s">
+      <c r="A7" s="11"/>
+      <c r="B7" s="11" t="s">
         <v>16</v>
       </c>
+      <c r="C7" s="11"/>
       <c r="D7" s="11"/>
       <c r="E7" s="4"/>
       <c r="F7" s="5"/>
@@ -1129,341 +1121,505 @@
         <v>13</v>
       </c>
     </row>
+    <row r="10" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>53</v>
+      </c>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
+      <c r="I10" s="11"/>
+      <c r="J10" s="11"/>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11"/>
+      <c r="M10" s="11"/>
+      <c r="N10" s="11"/>
+      <c r="O10" s="11"/>
+      <c r="P10" s="11"/>
+      <c r="Q10" s="11"/>
+      <c r="R10" s="11"/>
+      <c r="S10" s="11"/>
+      <c r="T10" s="11"/>
+    </row>
+    <row r="11" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="D11" s="11"/>
+      <c r="E11" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="F11" s="11"/>
+      <c r="G11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="H11" s="11"/>
+      <c r="I11" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="L11" s="11"/>
+      <c r="M11" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="N11" s="11"/>
+      <c r="O11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R11" s="11"/>
+      <c r="S11" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="T11" s="11"/>
+    </row>
+    <row r="12" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="12"/>
+      <c r="C12" s="25"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F12" s="12"/>
+      <c r="G12" s="25"/>
+      <c r="H12" s="10"/>
+      <c r="I12" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="J12" s="12"/>
+      <c r="K12" s="25"/>
+      <c r="L12" s="10"/>
+      <c r="M12" s="12" t="s">
+        <v>12</v>
+      </c>
+      <c r="N12" s="12"/>
+      <c r="O12" s="25"/>
+      <c r="P12" s="10"/>
+      <c r="Q12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="R12" s="12"/>
+      <c r="S12" s="25"/>
+      <c r="T12" s="10"/>
+      <c r="U12" s="23"/>
+      <c r="V12" s="23"/>
+      <c r="W12" s="23"/>
+      <c r="X12" s="23"/>
+      <c r="Y12" s="23"/>
+      <c r="Z12" s="23"/>
+    </row>
     <row r="13" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="F13" s="13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
-      <c r="I13" s="13"/>
-      <c r="J13" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="O13" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="S13" s="7" t="s">
-        <v>14</v>
-      </c>
-      <c r="T13" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="U13" s="13" t="s">
-        <v>24</v>
-      </c>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
-      <c r="Y13" s="13"/>
-      <c r="Z13" s="13" t="s">
-        <v>16</v>
-      </c>
+      <c r="A13" s="12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B13" s="12"/>
+      <c r="C13" s="12"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F13" s="12"/>
+      <c r="G13" s="12"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="12" t="s">
+        <v>51</v>
+      </c>
+      <c r="J13" s="12"/>
+      <c r="K13" s="12"/>
+      <c r="L13" s="9"/>
+      <c r="M13" s="12" t="s">
+        <v>38</v>
+      </c>
+      <c r="N13" s="12"/>
+      <c r="O13" s="12"/>
+      <c r="P13" s="9"/>
+      <c r="Q13" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="R13" s="12"/>
+      <c r="S13" s="12"/>
+      <c r="T13" s="9"/>
+      <c r="U13" s="23"/>
+      <c r="V13" s="23"/>
+      <c r="W13" s="23"/>
+      <c r="X13" s="23"/>
+      <c r="Y13" s="23"/>
+      <c r="Z13" s="23"/>
     </row>
     <row r="14" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="K14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="L14" s="7" t="s">
+      <c r="A14" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="B14" s="12"/>
+      <c r="C14" s="12"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="9"/>
+      <c r="I14" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="J14" s="12"/>
+      <c r="K14" s="12"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="M14" s="7" t="s">
+      <c r="N14" s="12"/>
+      <c r="O14" s="12"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="R14" s="12"/>
+      <c r="S14" s="12"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="23"/>
+      <c r="V14" s="23"/>
+      <c r="W14" s="23"/>
+      <c r="X14" s="23"/>
+      <c r="Y14" s="23"/>
+      <c r="Z14" s="23"/>
+    </row>
+    <row r="15" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B15" s="12"/>
+      <c r="C15" s="12"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="9"/>
+      <c r="I15" s="12" t="s">
+        <v>21</v>
+      </c>
+      <c r="J15" s="12"/>
+      <c r="K15" s="12"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="N15" s="12"/>
+      <c r="O15" s="12"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="R15" s="12"/>
+      <c r="S15" s="12"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="23"/>
+      <c r="V15" s="23"/>
+      <c r="W15" s="23"/>
+      <c r="X15" s="23"/>
+      <c r="Y15" s="23"/>
+      <c r="Z15" s="23"/>
+    </row>
+    <row r="16" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="12" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="12"/>
+      <c r="C16" s="12"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="12"/>
+      <c r="K16" s="12"/>
+      <c r="L16" s="9"/>
+      <c r="M16" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="U14" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="V14" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="W14" s="7" t="s">
-        <v>51</v>
-      </c>
-      <c r="X14" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="Y14" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="Z14" s="13"/>
-    </row>
-    <row r="15" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="F15" s="7" t="s">
-        <v>58</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="H15" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="I15" s="7" t="s">
-        <v>60</v>
-      </c>
-      <c r="J15" s="7" t="s">
+      <c r="N16" s="12"/>
+      <c r="O16" s="12"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="12"/>
+      <c r="R16" s="12"/>
+      <c r="S16" s="12"/>
+      <c r="T16" s="9"/>
+      <c r="U16" s="23"/>
+      <c r="V16" s="23"/>
+      <c r="W16" s="23"/>
+      <c r="X16" s="23"/>
+      <c r="Y16" s="23"/>
+      <c r="Z16" s="23"/>
+    </row>
+    <row r="17" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="B17" s="12"/>
+      <c r="C17" s="12"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="12" t="s">
         <v>52</v>
       </c>
-      <c r="K15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="L15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="N15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="S15" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="T15" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="U15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="V15" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="W15" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="X15" s="8" t="s">
-        <v>52</v>
-      </c>
-      <c r="Y15" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="16" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="K16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="M16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="N16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="T16" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="U16" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="V16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="W16" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="X16" s="8" t="s">
-        <v>57</v>
-      </c>
-      <c r="Y16" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="17" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="T17" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="U17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="V17" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="W17" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="18" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="K18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="L18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="T18" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="U18" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="V18" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="W18" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="21" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="I21" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="S21" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="T21" s="7" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I22" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="T22" s="7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I23" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="T23" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="S24" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="T24" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="I25" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="S25" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="T25" s="7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I26" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="T26" s="7" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="I27" s="7" t="s">
-        <v>23</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J28" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="U28" s="7" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="29" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J29" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="U29" s="7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J30" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="U30" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="31" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J31" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="U31" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="32" spans="1:23" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J32" s="7" t="s">
-        <v>47</v>
-      </c>
-      <c r="U32" s="7" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="33" spans="10:21" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J33" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="U33" s="7" t="s">
-        <v>48</v>
-      </c>
+      <c r="J17" s="12"/>
+      <c r="K17" s="12"/>
+      <c r="L17" s="9"/>
+      <c r="M17" s="12"/>
+      <c r="N17" s="12"/>
+      <c r="O17" s="12"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="12"/>
+      <c r="R17" s="12"/>
+      <c r="S17" s="12"/>
+      <c r="T17" s="9"/>
+      <c r="U17" s="23"/>
+      <c r="V17" s="23"/>
+      <c r="W17" s="23"/>
+      <c r="X17" s="23"/>
+      <c r="Y17" s="23"/>
+      <c r="Z17" s="23"/>
+    </row>
+    <row r="18" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S18" s="23"/>
+      <c r="T18" s="23"/>
+      <c r="U18" s="23"/>
+      <c r="V18" s="23"/>
+      <c r="W18" s="23"/>
+      <c r="X18" s="23"/>
+      <c r="Y18" s="23"/>
+      <c r="Z18" s="23"/>
+    </row>
+    <row r="19" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="T19" s="8"/>
+      <c r="U19" s="8"/>
+      <c r="V19" s="8"/>
+      <c r="X19" s="23"/>
+      <c r="Y19" s="23"/>
+      <c r="Z19" s="23"/>
+    </row>
+    <row r="20" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R20" s="8"/>
+      <c r="S20" s="8"/>
+      <c r="T20" s="8"/>
+      <c r="U20" s="8"/>
+      <c r="V20" s="8"/>
+      <c r="X20" s="23"/>
+      <c r="Y20" s="23"/>
+      <c r="Z20" s="23"/>
+    </row>
+    <row r="21" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R21" s="8"/>
+      <c r="S21" s="8"/>
+      <c r="T21" s="8"/>
+      <c r="X21" s="23"/>
+      <c r="Y21" s="23"/>
+      <c r="Z21" s="23"/>
+    </row>
+    <row r="22" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="R22" s="8"/>
+      <c r="S22" s="8"/>
+      <c r="T22" s="8"/>
+      <c r="X22" s="23"/>
+      <c r="Y22" s="23"/>
+      <c r="Z22" s="23"/>
+    </row>
+    <row r="23" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="X23" s="23"/>
+      <c r="Y23" s="23"/>
+      <c r="Z23" s="23"/>
+    </row>
+    <row r="24" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S24" s="23"/>
+      <c r="T24" s="23"/>
+      <c r="U24" s="23"/>
+      <c r="V24" s="23"/>
+      <c r="W24" s="23"/>
+      <c r="X24" s="23"/>
+      <c r="Y24" s="23"/>
+      <c r="Z24" s="23"/>
+    </row>
+    <row r="25" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="S25" s="23"/>
+      <c r="T25" s="23"/>
+      <c r="U25" s="23"/>
+      <c r="V25" s="23"/>
+      <c r="W25" s="23"/>
+      <c r="X25" s="23"/>
+      <c r="Y25" s="23"/>
+      <c r="Z25" s="23"/>
+    </row>
+    <row r="26" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W26" s="23"/>
+      <c r="X26" s="23"/>
+      <c r="Y26" s="23"/>
+      <c r="Z26" s="23"/>
+    </row>
+    <row r="27" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W27" s="23"/>
+      <c r="X27" s="23"/>
+      <c r="Y27" s="23"/>
+      <c r="Z27" s="23"/>
+    </row>
+    <row r="28" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W28" s="23"/>
+      <c r="X28" s="23"/>
+      <c r="Y28" s="23"/>
+      <c r="Z28" s="23"/>
+    </row>
+    <row r="29" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W29" s="23"/>
+      <c r="X29" s="23"/>
+      <c r="Y29" s="23"/>
+      <c r="Z29" s="23"/>
+    </row>
+    <row r="30" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W30" s="23"/>
+      <c r="X30" s="23"/>
+      <c r="Y30" s="23"/>
+      <c r="Z30" s="23"/>
+    </row>
+    <row r="31" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W31" s="23"/>
+      <c r="X31" s="23"/>
+      <c r="Y31" s="23"/>
+      <c r="Z31" s="23"/>
+    </row>
+    <row r="32" spans="1:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W32" s="23"/>
+      <c r="X32" s="23"/>
+      <c r="Y32" s="23"/>
+      <c r="Z32" s="23"/>
+    </row>
+    <row r="33" spans="23:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W33" s="23"/>
+      <c r="X33" s="23"/>
+      <c r="Y33" s="23"/>
+      <c r="Z33" s="23"/>
+    </row>
+    <row r="34" spans="23:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W34" s="23"/>
+      <c r="X34" s="23"/>
+      <c r="Y34" s="23"/>
+      <c r="Z34" s="23"/>
+    </row>
+    <row r="35" spans="23:26" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="W35" s="23"/>
+      <c r="X35" s="23"/>
+      <c r="Y35" s="23"/>
+      <c r="Z35" s="23"/>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="U13:Y13"/>
-    <mergeCell ref="Z13:Z14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C4:C6"/>
+  <mergeCells count="82">
+    <mergeCell ref="S16:T16"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="Q12:R12"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="Q14:R14"/>
+    <mergeCell ref="Q15:R15"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:B16"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="M11:N11"/>
+    <mergeCell ref="M12:N12"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="M14:N14"/>
+    <mergeCell ref="M15:N15"/>
+    <mergeCell ref="M16:N16"/>
+    <mergeCell ref="M17:N17"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E10:T10"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="E12:F12"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E15:F15"/>
+    <mergeCell ref="E16:F16"/>
+    <mergeCell ref="E17:F17"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="I14:J14"/>
+    <mergeCell ref="I15:J15"/>
+    <mergeCell ref="I16:J16"/>
+    <mergeCell ref="I17:J17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="K13:L13"/>
+    <mergeCell ref="K14:L14"/>
+    <mergeCell ref="K15:L15"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="O11:P11"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="O13:P13"/>
+    <mergeCell ref="O14:P14"/>
+    <mergeCell ref="O15:P15"/>
+    <mergeCell ref="O16:P16"/>
+    <mergeCell ref="O17:P17"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="Q16:R16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="B4:B6"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="A1:A7"/>
     <mergeCell ref="B1:B3"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="F13:I13"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1484,53 +1640,53 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:16" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="13" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="19"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="17"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="18"/>
     </row>
     <row r="2" spans="1:16" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15"/>
-      <c r="B2" s="20" t="s">
+      <c r="A2" s="14"/>
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="20" t="s">
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
+      <c r="E2" s="20"/>
+      <c r="F2" s="21"/>
+      <c r="G2" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="20" t="s">
+      <c r="H2" s="20"/>
+      <c r="I2" s="20"/>
+      <c r="J2" s="20"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="22"/>
+      <c r="M2" s="20"/>
+      <c r="N2" s="20"/>
+      <c r="O2" s="20"/>
+      <c r="P2" s="21"/>
     </row>
     <row r="3" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="16"/>
+      <c r="A3" s="15"/>
       <c r="B3" s="1" t="s">
         <v>3</v>
       </c>

</xml_diff>

<commit_message>
preparing for coding into an XML
</commit_message>
<xml_diff>
--- a/Documents/NecessaryDataForParser.xlsx
+++ b/Documents/NecessaryDataForParser.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="85">
   <si>
     <t>Место</t>
   </si>
@@ -63,9 +63,6 @@
     <t>Префикс</t>
   </si>
   <si>
-    <t>Постфикс</t>
-  </si>
-  <si>
     <t>после</t>
   </si>
   <si>
@@ -117,9 +114,18 @@
     <t>завтра</t>
   </si>
   <si>
+    <t>послезавтра</t>
+  </si>
+  <si>
+    <t>позавчера</t>
+  </si>
+  <si>
     <t>часов</t>
   </si>
   <si>
+    <t>*</t>
+  </si>
+  <si>
     <t>предыдущий</t>
   </si>
   <si>
@@ -150,12 +156,6 @@
     <t>воскресенье</t>
   </si>
   <si>
-    <t>~676</t>
-  </si>
-  <si>
-    <t>~8760</t>
-  </si>
-  <si>
     <t>++</t>
   </si>
   <si>
@@ -171,9 +171,6 @@
     <t>субботу</t>
   </si>
   <si>
-    <t>поза</t>
-  </si>
-  <si>
     <t>январь</t>
   </si>
   <si>
@@ -219,43 +216,13 @@
     <t>Описание</t>
   </si>
   <si>
-    <t>Паттерны</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">зависит от контекста, может использоваться как </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>префикс</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t xml:space="preserve">, имя, </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="8"/>
-        <color rgb="FF00B0F0"/>
-        <rFont val="Segoe UI"/>
-        <family val="2"/>
-        <charset val="204"/>
-      </rPr>
-      <t>постфикс</t>
-    </r>
+    <t>утро</t>
+  </si>
+  <si>
+    <t>вечер</t>
+  </si>
+  <si>
+    <t>ночь</t>
   </si>
   <si>
     <t xml:space="preserve"> </t>
@@ -273,17 +240,53 @@
     <t>прошлый</t>
   </si>
   <si>
-    <t>снгодя</t>
-  </si>
-  <si>
-    <t>составное</t>
+    <t>марте</t>
+  </si>
+  <si>
+    <t>вечером</t>
+  </si>
+  <si>
+    <t>TimeSpan</t>
+  </si>
+  <si>
+    <t>конкретный день, если не "сейчас"</t>
+  </si>
+  <si>
+    <t>по умолчанию 24h</t>
+  </si>
+  <si>
+    <t>по правилу</t>
+  </si>
+  <si>
+    <t>Паттерны + примеры</t>
+  </si>
+  <si>
+    <t>развёрнутое</t>
+  </si>
+  <si>
+    <t>известное</t>
+  </si>
+  <si>
+    <t>Всё, что наполучали, преобразуется к конкретному DateTime</t>
+  </si>
+  <si>
+    <t>1. Разбиваем на слова</t>
+  </si>
+  <si>
+    <t>3. Находим паттерн по последовательности маркеров</t>
+  </si>
+  <si>
+    <t>2. Ищем по словам маркеры (сравниваем с имеющимися, используя расстояние Дамерау-Левенштейна)</t>
+  </si>
+  <si>
+    <t>4. Выполняем соответствующую паттерну последовательность действий для заполнения DateTime</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -337,21 +340,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="8"/>
-      <color rgb="FF00B0F0"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF9C0006"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-      <charset val="204"/>
-    </font>
-    <font>
       <sz val="8"/>
       <color theme="1"/>
       <name val="Segoe UI"/>
@@ -360,6 +348,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="0"/>
+      <name val="Segoe UI"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color theme="0"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -392,12 +387,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -406,6 +395,12 @@
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
@@ -587,16 +582,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="48">
+  <cellXfs count="76">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -661,6 +655,12 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -682,6 +682,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -706,46 +715,114 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="1" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" xfId="6" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="10" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="2" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="1" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="3" xfId="3" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="11" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="15" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="12" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="10" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="2" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="13" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="9" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="14" xfId="5" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="7">
-    <cellStyle name="20% — акцент4" xfId="5" builtinId="42"/>
-    <cellStyle name="40% — акцент3" xfId="4" builtinId="39"/>
+  <cellStyles count="6">
+    <cellStyle name="20% — акцент4" xfId="4" builtinId="42"/>
     <cellStyle name="60% — акцент1" xfId="2" builtinId="32"/>
     <cellStyle name="60% — акцент2" xfId="3" builtinId="36"/>
-    <cellStyle name="60% — акцент6" xfId="6" builtinId="52"/>
+    <cellStyle name="60% — акцент6" xfId="5" builtinId="52"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
     <cellStyle name="Плохой" xfId="1" builtinId="27"/>
   </cellStyles>
@@ -1059,10 +1136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X32"/>
+  <dimension ref="A1:X34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J25" sqref="J25"/>
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.28515625" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1097,32 +1174,32 @@
     </row>
     <row r="2" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="16"/>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="57" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="37"/>
-      <c r="K2" s="37"/>
-      <c r="L2" s="37"/>
-      <c r="M2" s="37"/>
-      <c r="N2" s="37"/>
-      <c r="O2" s="37"/>
-      <c r="Q2" s="38" t="s">
-        <v>64</v>
-      </c>
-      <c r="R2" s="38"/>
-      <c r="S2" s="38"/>
-      <c r="T2" s="38"/>
-      <c r="U2" s="38"/>
-      <c r="V2" s="38"/>
-      <c r="W2" s="38"/>
-      <c r="X2" s="38"/>
+      <c r="C2" s="57"/>
+      <c r="D2" s="57"/>
+      <c r="E2" s="57"/>
+      <c r="F2" s="57"/>
+      <c r="G2" s="57"/>
+      <c r="H2" s="57"/>
+      <c r="I2" s="57"/>
+      <c r="J2" s="57"/>
+      <c r="K2" s="57"/>
+      <c r="L2" s="57"/>
+      <c r="M2" s="57"/>
+      <c r="N2" s="57"/>
+      <c r="O2" s="57"/>
+      <c r="Q2" s="56" t="s">
+        <v>77</v>
+      </c>
+      <c r="R2" s="56"/>
+      <c r="S2" s="56"/>
+      <c r="T2" s="56"/>
+      <c r="U2" s="56"/>
+      <c r="V2" s="56"/>
+      <c r="W2" s="56"/>
+      <c r="X2" s="56"/>
     </row>
     <row r="3" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16"/>
@@ -1132,557 +1209,875 @@
     </row>
     <row r="4" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="16"/>
-      <c r="B4" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="39"/>
+      <c r="B4" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="42"/>
       <c r="D4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E4" s="11"/>
-      <c r="G4" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="H4" s="40"/>
+      <c r="G4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="H4" s="43"/>
       <c r="I4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="J4" s="11"/>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="M4" s="41"/>
+      <c r="M4" s="44"/>
       <c r="N4" s="11" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="O4" s="11"/>
-      <c r="Q4" s="41" t="s">
-        <v>11</v>
-      </c>
-      <c r="R4" s="41"/>
-      <c r="S4" s="40" t="s">
-        <v>25</v>
-      </c>
-      <c r="T4" s="40"/>
-      <c r="U4" s="39" t="s">
-        <v>16</v>
-      </c>
-      <c r="V4" s="39"/>
-      <c r="W4" s="41" t="s">
-        <v>12</v>
-      </c>
-      <c r="X4" s="41"/>
+      <c r="Q4" s="11"/>
+      <c r="R4" s="11"/>
+      <c r="S4" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="T4" s="43"/>
+      <c r="U4" s="11"/>
+      <c r="V4" s="11"/>
+      <c r="W4" s="11"/>
+      <c r="X4" s="11"/>
     </row>
     <row r="5" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="16"/>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="35" t="s">
         <v>10</v>
       </c>
       <c r="C5" s="13"/>
-      <c r="D5" s="13">
-        <v>1</v>
+      <c r="D5" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="E5" s="14"/>
-      <c r="G5" s="30" t="s">
-        <v>31</v>
+      <c r="G5" s="35" t="s">
+        <v>33</v>
       </c>
       <c r="H5" s="13"/>
       <c r="I5" s="21" t="s">
         <v>45</v>
       </c>
       <c r="J5" s="14"/>
-      <c r="L5" s="30" t="s">
-        <v>17</v>
+      <c r="L5" s="35" t="s">
+        <v>16</v>
       </c>
       <c r="M5" s="13"/>
       <c r="N5" s="13"/>
       <c r="O5" s="14"/>
-      <c r="Q5" s="11" t="s">
-        <v>17</v>
-      </c>
+      <c r="Q5" s="11"/>
       <c r="R5" s="11"/>
-      <c r="S5" s="11">
-        <v>7</v>
-      </c>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11" t="s">
-        <v>30</v>
-      </c>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="S5" s="54" t="s">
+        <v>72</v>
+      </c>
+      <c r="T5" s="59"/>
+      <c r="U5" s="53" t="s">
+        <v>26</v>
+      </c>
+      <c r="V5" s="53"/>
+      <c r="W5" s="11"/>
       <c r="X5" s="11"/>
     </row>
     <row r="6" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="16"/>
-      <c r="B6" s="29" t="s">
-        <v>21</v>
+      <c r="B6" s="34" t="s">
+        <v>20</v>
       </c>
       <c r="C6" s="15"/>
-      <c r="D6" s="15">
-        <v>24</v>
-      </c>
+      <c r="D6" s="15"/>
       <c r="E6" s="17"/>
-      <c r="G6" s="29" t="s">
-        <v>32</v>
+      <c r="G6" s="34" t="s">
+        <v>34</v>
       </c>
       <c r="H6" s="15"/>
       <c r="I6" s="15">
         <v>0</v>
       </c>
       <c r="J6" s="17"/>
-      <c r="L6" s="29" t="s">
+      <c r="L6" s="34" t="s">
         <v>46</v>
       </c>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
       <c r="O6" s="17"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="15"/>
-      <c r="S6" s="15"/>
-      <c r="T6" s="15"/>
-      <c r="U6" s="15"/>
-      <c r="V6" s="15"/>
-      <c r="W6" s="15"/>
-      <c r="X6" s="15"/>
     </row>
     <row r="7" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="16"/>
-      <c r="B7" s="29" t="s">
-        <v>22</v>
+      <c r="B7" s="34" t="s">
+        <v>21</v>
       </c>
       <c r="C7" s="15"/>
-      <c r="D7" s="15">
-        <v>168</v>
-      </c>
+      <c r="D7" s="15"/>
       <c r="E7" s="17"/>
-      <c r="G7" s="29" t="s">
-        <v>20</v>
+      <c r="G7" s="34" t="s">
+        <v>19</v>
       </c>
       <c r="H7" s="15"/>
       <c r="I7" s="20" t="s">
         <v>43</v>
       </c>
       <c r="J7" s="17"/>
-      <c r="L7" s="29" t="s">
-        <v>18</v>
+      <c r="L7" s="34" t="s">
+        <v>17</v>
       </c>
       <c r="M7" s="15"/>
       <c r="N7" s="15"/>
       <c r="O7" s="17"/>
-      <c r="Q7" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="R7" s="42"/>
-      <c r="S7" s="43" t="s">
-        <v>25</v>
-      </c>
-      <c r="T7" s="43"/>
-      <c r="U7" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="V7" s="44"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="32"/>
+      <c r="S7" s="60"/>
+      <c r="T7" s="61"/>
+      <c r="U7" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="V7" s="42"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="33"/>
     </row>
     <row r="8" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="29" t="s">
-        <v>23</v>
+      <c r="B8" s="34" t="s">
+        <v>22</v>
       </c>
       <c r="C8" s="15"/>
-      <c r="D8" s="15" t="s">
-        <v>41</v>
-      </c>
+      <c r="D8" s="15"/>
       <c r="E8" s="17"/>
-      <c r="G8" s="29" t="s">
-        <v>14</v>
+      <c r="G8" s="34" t="s">
+        <v>13</v>
       </c>
       <c r="H8" s="15"/>
       <c r="I8" s="20" t="s">
         <v>44</v>
       </c>
       <c r="J8" s="17"/>
-      <c r="L8" s="29" t="s">
+      <c r="L8" s="34" t="s">
         <v>9</v>
       </c>
       <c r="M8" s="15"/>
       <c r="N8" s="15"/>
       <c r="O8" s="17"/>
-      <c r="Q8" s="30" t="s">
-        <v>18</v>
-      </c>
-      <c r="R8" s="14"/>
-      <c r="S8" s="30">
-        <v>28</v>
-      </c>
-      <c r="T8" s="14"/>
-      <c r="U8" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="V8" s="14"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="18"/>
+      <c r="S8" s="22"/>
+      <c r="T8" s="23"/>
+      <c r="U8" s="64" t="s">
+        <v>27</v>
+      </c>
+      <c r="V8" s="64"/>
+      <c r="W8" s="48">
+        <v>12</v>
+      </c>
+      <c r="X8" s="49"/>
     </row>
     <row r="9" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="28" t="s">
-        <v>24</v>
+      <c r="B9" s="30" t="s">
+        <v>23</v>
       </c>
       <c r="C9" s="18"/>
-      <c r="D9" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="E9" s="17"/>
-      <c r="G9" s="29" t="s">
-        <v>15</v>
+      <c r="D9" s="18"/>
+      <c r="E9" s="19"/>
+      <c r="G9" s="34" t="s">
+        <v>14</v>
       </c>
       <c r="H9" s="15"/>
       <c r="I9" s="20" t="s">
         <v>44</v>
       </c>
       <c r="J9" s="17"/>
-      <c r="L9" s="29" t="s">
-        <v>13</v>
-      </c>
-      <c r="M9" s="15"/>
-      <c r="N9" s="15"/>
-      <c r="O9" s="17"/>
-      <c r="Q9" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="R9" s="17"/>
-      <c r="S9" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="T9" s="17"/>
-      <c r="U9" s="15" t="s">
-        <v>37</v>
-      </c>
-      <c r="V9" s="17"/>
+      <c r="L9" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="M9" s="18"/>
+      <c r="N9" s="18"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="29" t="s">
-        <v>28</v>
-      </c>
-      <c r="C10" s="15"/>
-      <c r="D10" s="22" t="s">
+      <c r="B10" s="35" t="s">
+        <v>30</v>
+      </c>
+      <c r="C10" s="13"/>
+      <c r="D10" s="24" t="s">
+        <v>74</v>
+      </c>
+      <c r="E10" s="25"/>
+      <c r="G10" s="34" t="s">
         <v>65</v>
       </c>
-      <c r="E10" s="23"/>
-      <c r="G10" s="28" t="s">
-        <v>33</v>
-      </c>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="19"/>
-      <c r="L10" s="28" t="s">
-        <v>48</v>
-      </c>
-      <c r="M10" s="18"/>
-      <c r="N10" s="18"/>
-      <c r="O10" s="19"/>
-      <c r="Q10" s="28" t="s">
-        <v>9</v>
-      </c>
-      <c r="R10" s="19"/>
-      <c r="S10" s="28">
-        <v>4</v>
-      </c>
-      <c r="T10" s="19"/>
-      <c r="U10" s="18" t="s">
-        <v>69</v>
-      </c>
-      <c r="V10" s="19"/>
+      <c r="H10" s="15"/>
+      <c r="I10" s="15">
+        <v>0</v>
+      </c>
+      <c r="J10" s="17"/>
+      <c r="L10" s="16"/>
+      <c r="M10" s="16"/>
+      <c r="N10" s="16"/>
+      <c r="O10" s="16"/>
+      <c r="Q10" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="R10" s="45"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="33"/>
+      <c r="U10" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="V10" s="42"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="33"/>
     </row>
     <row r="11" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="29" t="s">
-        <v>26</v>
+      <c r="B11" s="34" t="s">
+        <v>27</v>
       </c>
       <c r="C11" s="15"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="25"/>
+      <c r="D11" s="26"/>
+      <c r="E11" s="27"/>
+      <c r="G11" s="34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="15"/>
+      <c r="I11" s="15">
+        <v>6</v>
+      </c>
+      <c r="J11" s="17"/>
+      <c r="Q11" s="62" t="s">
+        <v>16</v>
+      </c>
+      <c r="R11" s="63"/>
+      <c r="S11" s="62" t="s">
+        <v>76</v>
+      </c>
+      <c r="T11" s="63"/>
+      <c r="U11" s="51" t="s">
+        <v>71</v>
+      </c>
+      <c r="V11" s="52"/>
+      <c r="W11" s="35"/>
+      <c r="X11" s="14"/>
     </row>
     <row r="12" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="B12" s="29" t="s">
-        <v>27</v>
+      <c r="B12" s="34" t="s">
+        <v>25</v>
       </c>
       <c r="C12" s="15"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="25"/>
-      <c r="Q12" s="42" t="s">
-        <v>11</v>
-      </c>
-      <c r="R12" s="42"/>
-      <c r="S12" s="44" t="s">
-        <v>16</v>
-      </c>
-      <c r="T12" s="44"/>
+      <c r="D12" s="26"/>
+      <c r="E12" s="27"/>
+      <c r="G12" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" s="15"/>
+      <c r="I12" s="15">
+        <v>12</v>
+      </c>
+      <c r="J12" s="17"/>
+      <c r="Q12" s="34" t="s">
+        <v>17</v>
+      </c>
+      <c r="R12" s="17"/>
+      <c r="S12" s="34"/>
+      <c r="T12" s="17"/>
+      <c r="U12" s="34" t="s">
+        <v>26</v>
+      </c>
+      <c r="V12" s="17"/>
+      <c r="W12" s="34"/>
+      <c r="X12" s="17"/>
     </row>
     <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="29" t="s">
-        <v>29</v>
+      <c r="B13" s="34" t="s">
+        <v>26</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="26"/>
       <c r="E13" s="27"/>
-      <c r="Q13" s="30" t="s">
+      <c r="G13" s="34" t="s">
+        <v>64</v>
+      </c>
+      <c r="H13" s="15"/>
+      <c r="I13" s="15">
         <v>18</v>
       </c>
-      <c r="R13" s="14"/>
-      <c r="S13" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="T13" s="14"/>
+      <c r="J13" s="17"/>
+      <c r="Q13" s="34" t="s">
+        <v>12</v>
+      </c>
+      <c r="R13" s="17"/>
+      <c r="S13" s="34"/>
+      <c r="T13" s="17"/>
+      <c r="U13" s="34" t="s">
+        <v>13</v>
+      </c>
+      <c r="V13" s="17"/>
+      <c r="W13" s="34"/>
+      <c r="X13" s="17"/>
     </row>
     <row r="14" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="30" t="s">
-        <v>34</v>
-      </c>
-      <c r="C14" s="13"/>
-      <c r="D14" s="22" t="s">
-        <v>62</v>
-      </c>
-      <c r="E14" s="23"/>
-      <c r="Q14" s="29" t="s">
-        <v>18</v>
-      </c>
-      <c r="R14" s="17"/>
-      <c r="S14" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="T14" s="17"/>
+      <c r="B14" s="34" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="15"/>
+      <c r="D14" s="26"/>
+      <c r="E14" s="27"/>
+      <c r="G14" s="30" t="s">
+        <v>35</v>
+      </c>
+      <c r="H14" s="18"/>
+      <c r="I14" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="J14" s="19"/>
+      <c r="Q14" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="R14" s="49"/>
+      <c r="S14" s="48" t="s">
+        <v>76</v>
+      </c>
+      <c r="T14" s="49"/>
+      <c r="U14" s="48" t="s">
+        <v>47</v>
+      </c>
+      <c r="V14" s="49"/>
+      <c r="W14" s="30"/>
+      <c r="X14" s="19"/>
     </row>
     <row r="15" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="29" t="s">
-        <v>35</v>
-      </c>
-      <c r="C15" s="15"/>
-      <c r="D15" s="24"/>
-      <c r="E15" s="25"/>
-      <c r="P15" s="45" t="s">
-        <v>72</v>
-      </c>
-      <c r="Q15" s="46" t="s">
-        <v>13</v>
-      </c>
-      <c r="R15" s="47"/>
-      <c r="S15" s="46" t="s">
+      <c r="B15" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="T15" s="47"/>
+      <c r="C15" s="18"/>
+      <c r="D15" s="28"/>
+      <c r="E15" s="29"/>
     </row>
     <row r="16" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="29" t="s">
+      <c r="B16" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="C16" s="15"/>
-      <c r="D16" s="24"/>
+      <c r="C16" s="13"/>
+      <c r="D16" s="24" t="s">
+        <v>61</v>
+      </c>
       <c r="E16" s="25"/>
-      <c r="Q16" s="28" t="s">
+      <c r="G16" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="68"/>
+      <c r="I16" s="68"/>
+      <c r="J16" s="68"/>
+      <c r="K16" s="68"/>
+      <c r="L16" s="68"/>
+      <c r="M16" s="68"/>
+      <c r="N16" s="68"/>
+      <c r="O16" s="69"/>
+      <c r="Q16" s="45" t="s">
+        <v>11</v>
+      </c>
+      <c r="R16" s="45"/>
+      <c r="S16" s="46" t="s">
+        <v>24</v>
+      </c>
+      <c r="T16" s="46"/>
+      <c r="U16" s="47" t="s">
+        <v>15</v>
+      </c>
+      <c r="V16" s="47"/>
+      <c r="W16" s="31"/>
+      <c r="X16" s="33"/>
+    </row>
+    <row r="17" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="15"/>
+      <c r="D17" s="26"/>
+      <c r="E17" s="27"/>
+      <c r="G17" s="70"/>
+      <c r="H17" s="71"/>
+      <c r="I17" s="71"/>
+      <c r="J17" s="71"/>
+      <c r="K17" s="71"/>
+      <c r="L17" s="71"/>
+      <c r="M17" s="71"/>
+      <c r="N17" s="71"/>
+      <c r="O17" s="72"/>
+      <c r="Q17" s="35" t="s">
         <v>17</v>
       </c>
-      <c r="R16" s="19"/>
-      <c r="S16" s="28" t="s">
-        <v>47</v>
-      </c>
-      <c r="T16" s="19"/>
-    </row>
-    <row r="17" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="29" t="s">
-        <v>37</v>
-      </c>
-      <c r="C17" s="15"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-    </row>
-    <row r="18" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="29" t="s">
+      <c r="R17" s="14"/>
+      <c r="S17" s="35">
+        <v>28</v>
+      </c>
+      <c r="T17" s="14"/>
+      <c r="U17" s="13" t="s">
+        <v>67</v>
+      </c>
+      <c r="V17" s="14"/>
+      <c r="W17" s="65" t="s">
+        <v>79</v>
+      </c>
+      <c r="X17" s="14"/>
+    </row>
+    <row r="18" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="34" t="s">
         <v>38</v>
       </c>
       <c r="C18" s="15"/>
-      <c r="D18" s="24"/>
-      <c r="E18" s="25"/>
-    </row>
-    <row r="19" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="29" t="s">
+      <c r="D18" s="26"/>
+      <c r="E18" s="27"/>
+      <c r="G18" s="73"/>
+      <c r="H18" s="74"/>
+      <c r="I18" s="74"/>
+      <c r="J18" s="74"/>
+      <c r="K18" s="74"/>
+      <c r="L18" s="74"/>
+      <c r="M18" s="74"/>
+      <c r="N18" s="74"/>
+      <c r="O18" s="75"/>
+      <c r="Q18" s="34" t="s">
+        <v>16</v>
+      </c>
+      <c r="R18" s="17"/>
+      <c r="S18" s="34" t="s">
+        <v>70</v>
+      </c>
+      <c r="T18" s="17"/>
+      <c r="U18" s="15" t="s">
         <v>39</v>
       </c>
+      <c r="V18" s="15"/>
+      <c r="W18" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="X18" s="17"/>
+    </row>
+    <row r="19" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="34" t="s">
+        <v>39</v>
+      </c>
       <c r="C19" s="15"/>
-      <c r="D19" s="24"/>
-      <c r="E19" s="25"/>
-    </row>
-    <row r="20" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="28" t="s">
+      <c r="D19" s="26"/>
+      <c r="E19" s="27"/>
+      <c r="G19" s="35" t="s">
+        <v>81</v>
+      </c>
+      <c r="H19" s="13"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="13"/>
+      <c r="N19" s="13"/>
+      <c r="O19" s="14"/>
+      <c r="Q19" s="34" t="s">
+        <v>9</v>
+      </c>
+      <c r="R19" s="15"/>
+      <c r="S19" s="34">
+        <v>4</v>
+      </c>
+      <c r="T19" s="15"/>
+      <c r="U19" s="34" t="s">
+        <v>69</v>
+      </c>
+      <c r="V19" s="17"/>
+      <c r="W19" s="66"/>
+      <c r="X19" s="17"/>
+    </row>
+    <row r="20" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="34" t="s">
         <v>40</v>
       </c>
-      <c r="C20" s="18"/>
+      <c r="C20" s="15"/>
       <c r="D20" s="26"/>
       <c r="E20" s="27"/>
-    </row>
-    <row r="21" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="30" t="s">
+      <c r="G20" s="34"/>
+      <c r="H20" s="15"/>
+      <c r="I20" s="15"/>
+      <c r="J20" s="15"/>
+      <c r="K20" s="15"/>
+      <c r="L20" s="15"/>
+      <c r="M20" s="15"/>
+      <c r="N20" s="15"/>
+      <c r="O20" s="17"/>
+      <c r="Q20" s="48" t="s">
+        <v>16</v>
+      </c>
+      <c r="R20" s="49"/>
+      <c r="S20" s="48">
+        <v>11</v>
+      </c>
+      <c r="T20" s="49"/>
+      <c r="U20" s="50" t="s">
+        <v>31</v>
+      </c>
+      <c r="V20" s="49"/>
+      <c r="W20" s="48" t="s">
+        <v>75</v>
+      </c>
+      <c r="X20" s="49"/>
+    </row>
+    <row r="21" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="15"/>
+      <c r="D21" s="26"/>
+      <c r="E21" s="27"/>
+      <c r="G21" s="34" t="s">
+        <v>83</v>
+      </c>
+      <c r="H21" s="15"/>
+      <c r="I21" s="15"/>
+      <c r="J21" s="15"/>
+      <c r="K21" s="15"/>
+      <c r="L21" s="15"/>
+      <c r="M21" s="15"/>
+      <c r="N21" s="15"/>
+      <c r="O21" s="17"/>
+    </row>
+    <row r="22" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="18"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="29"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="15"/>
+      <c r="I22" s="15"/>
+      <c r="J22" s="15"/>
+      <c r="K22" s="15"/>
+      <c r="L22" s="15"/>
+      <c r="M22" s="15"/>
+      <c r="N22" s="15"/>
+      <c r="O22" s="17"/>
+      <c r="Q22" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="R22" s="44"/>
+      <c r="S22" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="T22" s="43"/>
+      <c r="U22" s="11"/>
+      <c r="V22" s="11"/>
+      <c r="W22" s="58"/>
+      <c r="X22" s="58"/>
+    </row>
+    <row r="23" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="13"/>
+      <c r="D23" s="36" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" s="37"/>
+      <c r="G23" s="34" t="s">
+        <v>82</v>
+      </c>
+      <c r="H23" s="15"/>
+      <c r="I23" s="15"/>
+      <c r="J23" s="15"/>
+      <c r="K23" s="15"/>
+      <c r="L23" s="15"/>
+      <c r="M23" s="15"/>
+      <c r="N23" s="15"/>
+      <c r="O23" s="17"/>
+      <c r="Q23" s="53" t="s">
+        <v>16</v>
+      </c>
+      <c r="R23" s="53"/>
+      <c r="S23" s="53">
+        <v>16</v>
+      </c>
+      <c r="T23" s="53"/>
+      <c r="U23" s="54"/>
+      <c r="V23" s="59"/>
+      <c r="W23" s="54" t="s">
+        <v>75</v>
+      </c>
+      <c r="X23" s="59"/>
+    </row>
+    <row r="24" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="13"/>
-      <c r="D21" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="E21" s="32"/>
-    </row>
-    <row r="22" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="29" t="s">
+      <c r="C24" s="15"/>
+      <c r="D24" s="38"/>
+      <c r="E24" s="39"/>
+      <c r="G24" s="34"/>
+      <c r="H24" s="15"/>
+      <c r="I24" s="15"/>
+      <c r="J24" s="15"/>
+      <c r="K24" s="15"/>
+      <c r="L24" s="15"/>
+      <c r="M24" s="15"/>
+      <c r="N24" s="15"/>
+      <c r="O24" s="17"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+    </row>
+    <row r="25" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="34" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="15"/>
-      <c r="D22" s="33"/>
-      <c r="E22" s="34"/>
-    </row>
-    <row r="23" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="29" t="s">
+      <c r="C25" s="15"/>
+      <c r="D25" s="38"/>
+      <c r="E25" s="39"/>
+      <c r="G25" s="34" t="s">
+        <v>84</v>
+      </c>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15"/>
+      <c r="J25" s="15"/>
+      <c r="K25" s="15"/>
+      <c r="L25" s="15"/>
+      <c r="M25" s="15"/>
+      <c r="N25" s="15"/>
+      <c r="O25" s="17"/>
+      <c r="Q25" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="R25" s="44"/>
+      <c r="S25" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="T25" s="43"/>
+      <c r="U25" s="42" t="s">
+        <v>15</v>
+      </c>
+      <c r="V25" s="42"/>
+      <c r="W25" s="43" t="s">
+        <v>24</v>
+      </c>
+      <c r="X25" s="43"/>
+    </row>
+    <row r="26" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="34" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="15"/>
-      <c r="D23" s="33"/>
-      <c r="E23" s="34"/>
-    </row>
-    <row r="24" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="29" t="s">
+      <c r="C26" s="15"/>
+      <c r="D26" s="38"/>
+      <c r="E26" s="39"/>
+      <c r="G26" s="30"/>
+      <c r="H26" s="18"/>
+      <c r="I26" s="18"/>
+      <c r="J26" s="18"/>
+      <c r="K26" s="18"/>
+      <c r="L26" s="18"/>
+      <c r="M26" s="18"/>
+      <c r="N26" s="18"/>
+      <c r="O26" s="19"/>
+      <c r="Q26" s="11" t="s">
+        <v>16</v>
+      </c>
+      <c r="R26" s="11"/>
+      <c r="S26" s="11">
+        <v>7</v>
+      </c>
+      <c r="T26" s="11"/>
+      <c r="U26" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="V26" s="11"/>
+      <c r="W26" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="X26" s="11"/>
+    </row>
+    <row r="27" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="34" t="s">
         <v>52</v>
       </c>
-      <c r="C24" s="15"/>
-      <c r="D24" s="33"/>
-      <c r="E24" s="34"/>
-    </row>
-    <row r="25" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="29" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="38"/>
+      <c r="E27" s="39"/>
+    </row>
+    <row r="28" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="34" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="15"/>
-      <c r="D25" s="33"/>
-      <c r="E25" s="34"/>
-    </row>
-    <row r="26" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
+      <c r="C28" s="15"/>
+      <c r="D28" s="38"/>
+      <c r="E28" s="39"/>
+    </row>
+    <row r="29" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="34" t="s">
         <v>54</v>
       </c>
-      <c r="C26" s="15"/>
-      <c r="D26" s="33"/>
-      <c r="E26" s="34"/>
-    </row>
-    <row r="27" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="29" t="s">
+      <c r="C29" s="15"/>
+      <c r="D29" s="38"/>
+      <c r="E29" s="39"/>
+    </row>
+    <row r="30" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="34" t="s">
         <v>55</v>
       </c>
-      <c r="C27" s="15"/>
-      <c r="D27" s="33"/>
-      <c r="E27" s="34"/>
-    </row>
-    <row r="28" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="29" t="s">
+      <c r="C30" s="15"/>
+      <c r="D30" s="38"/>
+      <c r="E30" s="39"/>
+    </row>
+    <row r="31" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="34" t="s">
         <v>56</v>
       </c>
-      <c r="C28" s="15"/>
-      <c r="D28" s="33"/>
-      <c r="E28" s="34"/>
-    </row>
-    <row r="29" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="29" t="s">
+      <c r="C31" s="15"/>
+      <c r="D31" s="38"/>
+      <c r="E31" s="39"/>
+    </row>
+    <row r="32" spans="2:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B32" s="34" t="s">
         <v>57</v>
       </c>
-      <c r="C29" s="15"/>
-      <c r="D29" s="33"/>
-      <c r="E29" s="34"/>
-    </row>
-    <row r="30" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="29" t="s">
+      <c r="C32" s="15"/>
+      <c r="D32" s="38"/>
+      <c r="E32" s="39"/>
+    </row>
+    <row r="33" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="34" t="s">
         <v>58</v>
       </c>
-      <c r="C30" s="15"/>
-      <c r="D30" s="33"/>
-      <c r="E30" s="34"/>
-    </row>
-    <row r="31" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="29" t="s">
+      <c r="C33" s="15"/>
+      <c r="D33" s="38"/>
+      <c r="E33" s="39"/>
+    </row>
+    <row r="34" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B34" s="30" t="s">
         <v>59</v>
       </c>
-      <c r="C31" s="15"/>
-      <c r="D31" s="33"/>
-      <c r="E31" s="34"/>
-    </row>
-    <row r="32" spans="2:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="28" t="s">
-        <v>60</v>
-      </c>
-      <c r="C32" s="18"/>
-      <c r="D32" s="35"/>
-      <c r="E32" s="36"/>
+      <c r="C34" s="18"/>
+      <c r="D34" s="40"/>
+      <c r="E34" s="41"/>
     </row>
   </sheetData>
-  <mergeCells count="99">
+  <mergeCells count="149">
+    <mergeCell ref="G16:O18"/>
+    <mergeCell ref="G19:O20"/>
+    <mergeCell ref="G23:O24"/>
+    <mergeCell ref="G25:O26"/>
+    <mergeCell ref="G21:O22"/>
+    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U22:V22"/>
+    <mergeCell ref="W16:X16"/>
+    <mergeCell ref="W17:X17"/>
+    <mergeCell ref="W18:X18"/>
+    <mergeCell ref="W19:X19"/>
+    <mergeCell ref="W14:X14"/>
+    <mergeCell ref="Q19:R19"/>
+    <mergeCell ref="W23:X23"/>
+    <mergeCell ref="W20:X20"/>
+    <mergeCell ref="Q22:R22"/>
+    <mergeCell ref="S22:T22"/>
+    <mergeCell ref="W22:X22"/>
+    <mergeCell ref="U23:V23"/>
+    <mergeCell ref="U13:V13"/>
+    <mergeCell ref="D5:E9"/>
+    <mergeCell ref="U7:V7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="S10:T10"/>
+    <mergeCell ref="S11:T11"/>
+    <mergeCell ref="S12:T12"/>
+    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="Q7:R7"/>
+    <mergeCell ref="Q8:R8"/>
+    <mergeCell ref="S7:T7"/>
+    <mergeCell ref="S8:T8"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="Q13:R13"/>
+    <mergeCell ref="W10:X10"/>
+    <mergeCell ref="W11:X11"/>
+    <mergeCell ref="W12:X12"/>
+    <mergeCell ref="W13:X13"/>
+    <mergeCell ref="W7:X7"/>
+    <mergeCell ref="W8:X8"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="U5:V5"/>
     <mergeCell ref="B2:O2"/>
+    <mergeCell ref="Q20:R20"/>
+    <mergeCell ref="S20:T20"/>
+    <mergeCell ref="U20:V20"/>
+    <mergeCell ref="Q18:R18"/>
+    <mergeCell ref="S18:T18"/>
+    <mergeCell ref="U18:V18"/>
     <mergeCell ref="Q10:R10"/>
-    <mergeCell ref="S10:T10"/>
     <mergeCell ref="U10:V10"/>
-    <mergeCell ref="Q9:R9"/>
-    <mergeCell ref="S9:T9"/>
-    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="Q11:R11"/>
+    <mergeCell ref="U11:V11"/>
     <mergeCell ref="Q12:R12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="Q13:R13"/>
-    <mergeCell ref="S13:T13"/>
+    <mergeCell ref="U12:V12"/>
     <mergeCell ref="Q14:R14"/>
-    <mergeCell ref="S14:T14"/>
+    <mergeCell ref="U14:V14"/>
     <mergeCell ref="Q16:R16"/>
     <mergeCell ref="S16:T16"/>
-    <mergeCell ref="Q7:R7"/>
-    <mergeCell ref="S7:T7"/>
-    <mergeCell ref="U7:V7"/>
-    <mergeCell ref="Q8:R8"/>
-    <mergeCell ref="S8:T8"/>
-    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="U16:V16"/>
+    <mergeCell ref="Q17:R17"/>
+    <mergeCell ref="S17:T17"/>
+    <mergeCell ref="U17:V17"/>
+    <mergeCell ref="W26:X26"/>
+    <mergeCell ref="Q25:R25"/>
+    <mergeCell ref="Q2:X2"/>
+    <mergeCell ref="S25:T25"/>
+    <mergeCell ref="U25:V25"/>
+    <mergeCell ref="W25:X25"/>
+    <mergeCell ref="D10:E15"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="I12:J12"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="W4:X4"/>
     <mergeCell ref="W5:X5"/>
-    <mergeCell ref="Q6:X6"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="Q2:X2"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="D10:E13"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="D21:E32"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="D23:E34"/>
     <mergeCell ref="B30:C30"/>
     <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
     <mergeCell ref="L6:M6"/>
-    <mergeCell ref="B21:C21"/>
-    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="B10:C10"/>
+    <mergeCell ref="G11:H11"/>
     <mergeCell ref="B23:C23"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="D14:E20"/>
-    <mergeCell ref="B14:C14"/>
-    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="Q26:R26"/>
+    <mergeCell ref="S26:T26"/>
+    <mergeCell ref="U26:V26"/>
+    <mergeCell ref="B22:C22"/>
+    <mergeCell ref="D16:E22"/>
+    <mergeCell ref="U19:V19"/>
     <mergeCell ref="B16:C16"/>
     <mergeCell ref="B17:C17"/>
     <mergeCell ref="B18:C18"/>
     <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="B21:C21"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B14:C14"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B11:C11"/>
     <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B10:C10"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="I14:J14"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="B8:C8"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="I10:J10"/>
     <mergeCell ref="D4:E4"/>
     <mergeCell ref="L4:M4"/>
     <mergeCell ref="N4:O4"/>
@@ -1690,30 +2085,24 @@
     <mergeCell ref="L7:M7"/>
     <mergeCell ref="L8:M8"/>
     <mergeCell ref="L9:M9"/>
-    <mergeCell ref="L10:M10"/>
     <mergeCell ref="G4:H4"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="G6:H6"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="G8:H8"/>
     <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G14:H14"/>
     <mergeCell ref="N8:O8"/>
     <mergeCell ref="N9:O9"/>
-    <mergeCell ref="N10:O10"/>
     <mergeCell ref="I4:J4"/>
     <mergeCell ref="I5:J5"/>
     <mergeCell ref="I6:J6"/>
     <mergeCell ref="I7:J7"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="Q15:R15"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="S15:T15"/>
+    <mergeCell ref="Q23:R23"/>
+    <mergeCell ref="S23:T23"/>
+    <mergeCell ref="S19:T19"/>
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="N6:O6"/>
     <mergeCell ref="N7:O7"/>

</xml_diff>

<commit_message>
added: Locations.xml, until can be loaded from the real Weather database
</commit_message>
<xml_diff>
--- a/Documents/NecessaryDataForParser.xlsx
+++ b/Documents/NecessaryDataForParser.xlsx
@@ -743,7 +743,7 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -860,9 +860,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="3" borderId="8" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="1" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="6" xfId="4" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1221,8 +1218,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:Y98"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="S40" sqref="S40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.85546875" defaultRowHeight="18" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1284,14 +1281,14 @@
       </c>
       <c r="I4" s="35"/>
       <c r="J4" s="36"/>
-      <c r="L4" s="41" t="s">
+      <c r="L4" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="42"/>
-      <c r="N4" s="42"/>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="43"/>
+      <c r="M4" s="41"/>
+      <c r="N4" s="41"/>
+      <c r="O4" s="41"/>
+      <c r="P4" s="41"/>
+      <c r="Q4" s="42"/>
       <c r="R4" s="32"/>
       <c r="S4" s="27" t="s">
         <v>8</v>
@@ -1324,16 +1321,16 @@
       <c r="M5" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="N5" s="47" t="s">
+      <c r="N5" s="46" t="s">
         <v>128</v>
       </c>
       <c r="O5" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="P5" s="40" t="s">
-        <v>128</v>
-      </c>
-      <c r="Q5" s="47" t="s">
+      <c r="P5" s="46" t="s">
+        <v>8</v>
+      </c>
+      <c r="Q5" s="46" t="s">
         <v>87</v>
       </c>
       <c r="R5" s="31"/>
@@ -1343,10 +1340,10 @@
       <c r="T5" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="U5" s="47" t="s">
+      <c r="U5" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="V5" s="47" t="s">
+      <c r="V5" s="46" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1531,14 +1528,14 @@
       <c r="N12" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="S12" s="41" t="s">
+      <c r="S12" s="40" t="s">
         <v>8</v>
       </c>
-      <c r="T12" s="42"/>
-      <c r="U12" s="42"/>
-      <c r="V12" s="42"/>
-      <c r="W12" s="42"/>
-      <c r="X12" s="43"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="42"/>
     </row>
     <row r="13" spans="1:24" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="34" t="s">
@@ -1569,10 +1566,10 @@
       <c r="T13" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="U13" s="47" t="s">
+      <c r="U13" s="46" t="s">
         <v>128</v>
       </c>
-      <c r="V13" s="47" t="s">
+      <c r="V13" s="46" t="s">
         <v>87</v>
       </c>
     </row>
@@ -1798,24 +1795,24 @@
       </c>
       <c r="I23" s="12"/>
       <c r="J23" s="13"/>
-      <c r="L23" s="50" t="s">
+      <c r="L23" s="49" t="s">
         <v>136</v>
       </c>
-      <c r="M23" s="51"/>
-      <c r="N23" s="51"/>
-      <c r="O23" s="51"/>
-      <c r="P23" s="52"/>
-      <c r="Q23" s="50" t="s">
+      <c r="M23" s="50"/>
+      <c r="N23" s="50"/>
+      <c r="O23" s="50"/>
+      <c r="P23" s="51"/>
+      <c r="Q23" s="49" t="s">
         <v>135</v>
       </c>
-      <c r="R23" s="51"/>
-      <c r="S23" s="51"/>
-      <c r="T23" s="52"/>
-      <c r="U23" s="50" t="s">
+      <c r="R23" s="50"/>
+      <c r="S23" s="50"/>
+      <c r="T23" s="51"/>
+      <c r="U23" s="49" t="s">
         <v>134</v>
       </c>
-      <c r="V23" s="51"/>
-      <c r="W23" s="52"/>
+      <c r="V23" s="50"/>
+      <c r="W23" s="51"/>
     </row>
     <row r="24" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="25" t="s">
@@ -1877,10 +1874,10 @@
       </c>
       <c r="Q26" s="35"/>
       <c r="R26" s="36"/>
-      <c r="T26" s="44" t="s">
+      <c r="T26" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="U26" s="46"/>
+      <c r="U26" s="45"/>
       <c r="V26" s="19" t="s">
         <v>79</v>
       </c>
@@ -2010,10 +2007,10 @@
       </c>
       <c r="Q30" s="16"/>
       <c r="R30" s="17"/>
-      <c r="T30" s="44" t="s">
+      <c r="T30" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="U30" s="46"/>
+      <c r="U30" s="45"/>
       <c r="V30" s="19" t="s">
         <v>79</v>
       </c>
@@ -2152,16 +2149,16 @@
       <c r="Y35" s="15"/>
     </row>
     <row r="36" spans="2:25" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="44" t="s">
+      <c r="B36" s="43" t="s">
         <v>123</v>
       </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="46"/>
-      <c r="F36" s="44" t="s">
+      <c r="C36" s="44"/>
+      <c r="D36" s="45"/>
+      <c r="F36" s="43" t="s">
         <v>126</v>
       </c>
-      <c r="G36" s="45"/>
-      <c r="H36" s="46"/>
+      <c r="G36" s="44"/>
+      <c r="H36" s="45"/>
       <c r="T36" s="25" t="s">
         <v>83</v>
       </c>
@@ -2254,92 +2251,92 @@
       <c r="H41" s="17"/>
     </row>
     <row r="88" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="48"/>
-      <c r="C88" s="48"/>
-      <c r="D88" s="48"/>
-      <c r="E88" s="48"/>
-      <c r="F88" s="48"/>
-      <c r="G88" s="48"/>
+      <c r="B88" s="47"/>
+      <c r="C88" s="47"/>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="47"/>
+      <c r="G88" s="47"/>
     </row>
     <row r="89" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B89" s="48"/>
-      <c r="C89" s="48"/>
-      <c r="D89" s="48"/>
-      <c r="E89" s="48"/>
-      <c r="F89" s="48"/>
-      <c r="G89" s="48"/>
+      <c r="B89" s="47"/>
+      <c r="C89" s="47"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="47"/>
+      <c r="G89" s="47"/>
     </row>
     <row r="90" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B90" s="48"/>
-      <c r="C90" s="48"/>
-      <c r="D90" s="48"/>
-      <c r="E90" s="48"/>
-      <c r="F90" s="48"/>
-      <c r="G90" s="48"/>
+      <c r="B90" s="47"/>
+      <c r="C90" s="47"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="47"/>
+      <c r="G90" s="47"/>
     </row>
     <row r="91" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B91" s="49"/>
-      <c r="C91" s="49"/>
-      <c r="D91" s="49"/>
-      <c r="E91" s="49"/>
-      <c r="F91" s="49"/>
-      <c r="G91" s="49"/>
+      <c r="B91" s="48"/>
+      <c r="C91" s="48"/>
+      <c r="D91" s="48"/>
+      <c r="E91" s="48"/>
+      <c r="F91" s="48"/>
+      <c r="G91" s="48"/>
     </row>
     <row r="92" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B92" s="49"/>
-      <c r="C92" s="49"/>
-      <c r="D92" s="49"/>
-      <c r="E92" s="49"/>
-      <c r="F92" s="49"/>
-      <c r="G92" s="49"/>
+      <c r="B92" s="48"/>
+      <c r="C92" s="48"/>
+      <c r="D92" s="48"/>
+      <c r="E92" s="48"/>
+      <c r="F92" s="48"/>
+      <c r="G92" s="48"/>
     </row>
     <row r="93" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B93" s="49"/>
-      <c r="C93" s="49"/>
-      <c r="D93" s="49"/>
-      <c r="E93" s="49"/>
-      <c r="F93" s="49"/>
-      <c r="G93" s="49"/>
+      <c r="B93" s="48"/>
+      <c r="C93" s="48"/>
+      <c r="D93" s="48"/>
+      <c r="E93" s="48"/>
+      <c r="F93" s="48"/>
+      <c r="G93" s="48"/>
     </row>
     <row r="94" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B94" s="49"/>
-      <c r="C94" s="49"/>
-      <c r="D94" s="49"/>
-      <c r="E94" s="49"/>
-      <c r="F94" s="49"/>
-      <c r="G94" s="49"/>
+      <c r="B94" s="48"/>
+      <c r="C94" s="48"/>
+      <c r="D94" s="48"/>
+      <c r="E94" s="48"/>
+      <c r="F94" s="48"/>
+      <c r="G94" s="48"/>
     </row>
     <row r="95" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B95" s="49"/>
-      <c r="C95" s="49"/>
-      <c r="D95" s="49"/>
-      <c r="E95" s="49"/>
-      <c r="F95" s="49"/>
-      <c r="G95" s="49"/>
+      <c r="B95" s="48"/>
+      <c r="C95" s="48"/>
+      <c r="D95" s="48"/>
+      <c r="E95" s="48"/>
+      <c r="F95" s="48"/>
+      <c r="G95" s="48"/>
     </row>
     <row r="96" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B96" s="49"/>
-      <c r="C96" s="49"/>
-      <c r="D96" s="49"/>
-      <c r="E96" s="49"/>
-      <c r="F96" s="49"/>
-      <c r="G96" s="49"/>
+      <c r="B96" s="48"/>
+      <c r="C96" s="48"/>
+      <c r="D96" s="48"/>
+      <c r="E96" s="48"/>
+      <c r="F96" s="48"/>
+      <c r="G96" s="48"/>
     </row>
     <row r="97" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B97" s="49"/>
-      <c r="C97" s="49"/>
-      <c r="D97" s="49"/>
-      <c r="E97" s="49"/>
-      <c r="F97" s="49"/>
-      <c r="G97" s="49"/>
+      <c r="B97" s="48"/>
+      <c r="C97" s="48"/>
+      <c r="D97" s="48"/>
+      <c r="E97" s="48"/>
+      <c r="F97" s="48"/>
+      <c r="G97" s="48"/>
     </row>
     <row r="98" spans="2:7" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B98" s="49"/>
-      <c r="C98" s="49"/>
-      <c r="D98" s="49"/>
-      <c r="E98" s="49"/>
-      <c r="F98" s="49"/>
-      <c r="G98" s="49"/>
+      <c r="B98" s="48"/>
+      <c r="C98" s="48"/>
+      <c r="D98" s="48"/>
+      <c r="E98" s="48"/>
+      <c r="F98" s="48"/>
+      <c r="G98" s="48"/>
     </row>
   </sheetData>
   <mergeCells count="143">

</xml_diff>